<commit_message>
Updated FIN model - 2025-08-25 16:59
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN/BY_Trans.xlsx
+++ b/VerveStacks_FIN/BY_Trans.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6F6923-CF0C-4E28-BDDF-F4AB3905A1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175BD090-9177-48E9-AFCC-2E73ABFECA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="misc." sheetId="2" r:id="rId1"/>
     <sheet name="pumped hydro" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>attribute</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t>-af</t>
+  </si>
+  <si>
+    <t>flo_emis</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>co2captured</t>
+  </si>
+  <si>
+    <t>co2</t>
+  </si>
+  <si>
+    <t>*ccs,*ccs-rf</t>
+  </si>
+  <si>
+    <t>coal,oil</t>
   </si>
 </sst>
 </file>
@@ -575,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982CB9B3-DA63-443B-9AA5-BEE16CBC2D59}">
-  <dimension ref="B3:J10"/>
+  <dimension ref="B3:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -586,17 +604,18 @@
     <col min="2" max="2" width="9.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.53125" customWidth="1"/>
     <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.53125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:12" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,8 +643,14 @@
       <c r="J4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -642,7 +667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -653,7 +678,7 @@
         <v>8.76</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -670,7 +695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -690,7 +715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -704,7 +729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>41</v>
       </c>
@@ -716,6 +741,46 @@
       </c>
       <c r="H10">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11">
+        <v>0.95</v>
+      </c>
+      <c r="K11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12">
+        <v>0.85</v>
+      </c>
+      <c r="K12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>